<commit_message>
Registo semanal update Semana 4 + Diagrama de Gantt v1.0
</commit_message>
<xml_diff>
--- a/doc/PEI-gantt.xlsx
+++ b/doc/PEI-gantt.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23930"/>
   <workbookPr dateCompatibility="0" filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6F9AAEE-9725-409E-8502-A6B7FB30EEED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF341EF9-1920-4611-ADE5-70AC59BCAA2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="101" uniqueCount="79">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="99" uniqueCount="79">
   <si>
     <t>Enter the name of the Project Lead in cell B3. Enter the Project Start date in cell E3. Pooject Start: label is in cell C3.</t>
   </si>
@@ -137,13 +137,19 @@
 Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more.</t>
   </si>
   <si>
-    <t>Implementação do esboço inicial do módulo Kafka e sua interligação com outros componentes</t>
-  </si>
-  <si>
-    <t>Correção de erros e revisão à implementação inicial</t>
-  </si>
-  <si>
-    <t>Preparação e interligação com APIs</t>
+    <t>Interligação e criação de uma aplicação exemplo com consumidores e produtores kafka</t>
+  </si>
+  <si>
+    <t>João Gameiro</t>
+  </si>
+  <si>
+    <t>Estudo e tentativa de implementação de um kafka broker numa máquina virtual</t>
+  </si>
+  <si>
+    <t>Pedro Abreu</t>
+  </si>
+  <si>
+    <t>Implementação do esboço inicial do módulo kafka</t>
   </si>
   <si>
     <t>Estudo para optimizações e preparação de módulo para o protótipo do sistema</t>
@@ -238,12 +244,6 @@
   </si>
   <si>
     <t>Estudo de máquinas virtuais na Azure para implementação do Módulo Kafka</t>
-  </si>
-  <si>
-    <t>Pedro Abreu</t>
-  </si>
-  <si>
-    <t>Estudo de APIs públicas para simulação de recolha de dados para efeitos de implementação inicial do sistema</t>
   </si>
   <si>
     <t>Backoffice</t>
@@ -770,7 +770,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1036,9 +1036,6 @@
     <xf numFmtId="168" fontId="8" fillId="15" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1051,6 +1048,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="20" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1063,13 +1067,6 @@
     <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="9" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1637,11 +1634,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL44"/>
+  <dimension ref="A1:BL43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -1665,341 +1662,341 @@
       <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="104" t="s">
+      <c r="C1" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="105"/>
-      <c r="E1" s="103" t="d">
+      <c r="D1" s="100"/>
+      <c r="E1" s="105" t="d">
         <v>2021-03-10</v>
       </c>
-      <c r="F1" s="103"/>
+      <c r="F1" s="105"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1">
       <c r="A2" s="43" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="66"/>
-      <c r="C2" s="104" t="s">
+      <c r="C2" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="105"/>
-      <c r="E2" s="99">
-        <v>3</v>
-      </c>
-      <c r="I2" s="100" t="d">
+      <c r="D2" s="100"/>
+      <c r="E2" s="98">
+        <v>5</v>
+      </c>
+      <c r="I2" s="102" t="d">
         <f>I3</f>
-        <v>2021-03-22</v>
-      </c>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="102"/>
-      <c r="P2" s="100" t="d">
+        <v>2021-04-05</v>
+      </c>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="102" t="d">
         <f>P3</f>
-        <v>2021-03-29</v>
-      </c>
-      <c r="Q2" s="101"/>
-      <c r="R2" s="101"/>
-      <c r="S2" s="101"/>
-      <c r="T2" s="101"/>
-      <c r="U2" s="101"/>
-      <c r="V2" s="102"/>
-      <c r="W2" s="100" t="d">
+        <v>2021-04-12</v>
+      </c>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="103"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="103"/>
+      <c r="V2" s="104"/>
+      <c r="W2" s="102" t="d">
         <f>W3</f>
-        <v>2021-04-05</v>
-      </c>
-      <c r="X2" s="101"/>
-      <c r="Y2" s="101"/>
-      <c r="Z2" s="101"/>
-      <c r="AA2" s="101"/>
-      <c r="AB2" s="101"/>
-      <c r="AC2" s="102"/>
-      <c r="AD2" s="100" t="d">
+        <v>2021-04-19</v>
+      </c>
+      <c r="X2" s="103"/>
+      <c r="Y2" s="103"/>
+      <c r="Z2" s="103"/>
+      <c r="AA2" s="103"/>
+      <c r="AB2" s="103"/>
+      <c r="AC2" s="104"/>
+      <c r="AD2" s="102" t="d">
         <f>AD3</f>
-        <v>2021-04-12</v>
-      </c>
-      <c r="AE2" s="101"/>
-      <c r="AF2" s="101"/>
-      <c r="AG2" s="101"/>
-      <c r="AH2" s="101"/>
-      <c r="AI2" s="101"/>
-      <c r="AJ2" s="102"/>
-      <c r="AK2" s="100" t="d">
+        <v>2021-04-26</v>
+      </c>
+      <c r="AE2" s="103"/>
+      <c r="AF2" s="103"/>
+      <c r="AG2" s="103"/>
+      <c r="AH2" s="103"/>
+      <c r="AI2" s="103"/>
+      <c r="AJ2" s="104"/>
+      <c r="AK2" s="102" t="d">
         <f>AK3</f>
-        <v>2021-04-19</v>
-      </c>
-      <c r="AL2" s="101"/>
-      <c r="AM2" s="101"/>
-      <c r="AN2" s="101"/>
-      <c r="AO2" s="101"/>
-      <c r="AP2" s="101"/>
-      <c r="AQ2" s="102"/>
-      <c r="AR2" s="100" t="d">
+        <v>2021-05-03</v>
+      </c>
+      <c r="AL2" s="103"/>
+      <c r="AM2" s="103"/>
+      <c r="AN2" s="103"/>
+      <c r="AO2" s="103"/>
+      <c r="AP2" s="103"/>
+      <c r="AQ2" s="104"/>
+      <c r="AR2" s="102" t="d">
         <f>AR3</f>
-        <v>2021-04-26</v>
-      </c>
-      <c r="AS2" s="101"/>
-      <c r="AT2" s="101"/>
-      <c r="AU2" s="101"/>
-      <c r="AV2" s="101"/>
-      <c r="AW2" s="101"/>
-      <c r="AX2" s="102"/>
-      <c r="AY2" s="100" t="d">
+        <v>2021-05-10</v>
+      </c>
+      <c r="AS2" s="103"/>
+      <c r="AT2" s="103"/>
+      <c r="AU2" s="103"/>
+      <c r="AV2" s="103"/>
+      <c r="AW2" s="103"/>
+      <c r="AX2" s="104"/>
+      <c r="AY2" s="102" t="d">
         <f>AY3</f>
-        <v>2021-05-03</v>
-      </c>
-      <c r="AZ2" s="101"/>
-      <c r="BA2" s="101"/>
-      <c r="BB2" s="101"/>
-      <c r="BC2" s="101"/>
-      <c r="BD2" s="101"/>
-      <c r="BE2" s="102"/>
-      <c r="BF2" s="100" t="d">
+        <v>2021-05-17</v>
+      </c>
+      <c r="AZ2" s="103"/>
+      <c r="BA2" s="103"/>
+      <c r="BB2" s="103"/>
+      <c r="BC2" s="103"/>
+      <c r="BD2" s="103"/>
+      <c r="BE2" s="104"/>
+      <c r="BF2" s="102" t="d">
         <f>BF3</f>
-        <v>2021-05-10</v>
-      </c>
-      <c r="BG2" s="101"/>
-      <c r="BH2" s="101"/>
-      <c r="BI2" s="101"/>
-      <c r="BJ2" s="101"/>
-      <c r="BK2" s="101"/>
-      <c r="BL2" s="102"/>
+        <v>2021-05-24</v>
+      </c>
+      <c r="BG2" s="103"/>
+      <c r="BH2" s="103"/>
+      <c r="BI2" s="103"/>
+      <c r="BJ2" s="103"/>
+      <c r="BK2" s="103"/>
+      <c r="BL2" s="104"/>
     </row>
     <row r="3" spans="1:64" ht="15" customHeight="1">
       <c r="A3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
       <c r="I3" s="59" t="d">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>2021-03-22</v>
+        <v>2021-04-05</v>
       </c>
       <c r="J3" s="60" t="d">
         <f>I3+1</f>
-        <v>2021-03-23</v>
+        <v>2021-04-06</v>
       </c>
       <c r="K3" s="60" t="d">
         <f t="shared" ref="K3:AX3" si="0">J3+1</f>
-        <v>2021-03-24</v>
+        <v>2021-04-07</v>
       </c>
       <c r="L3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-03-25</v>
+        <v>2021-04-08</v>
       </c>
       <c r="M3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-03-26</v>
+        <v>2021-04-09</v>
       </c>
       <c r="N3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-03-27</v>
+        <v>2021-04-10</v>
       </c>
       <c r="O3" s="61" t="d">
         <f t="shared" si="0"/>
-        <v>2021-03-28</v>
+        <v>2021-04-11</v>
       </c>
       <c r="P3" s="59" t="d">
         <f>O3+1</f>
-        <v>2021-03-29</v>
+        <v>2021-04-12</v>
       </c>
       <c r="Q3" s="60" t="d">
         <f>P3+1</f>
-        <v>2021-03-30</v>
+        <v>2021-04-13</v>
       </c>
       <c r="R3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-03-31</v>
+        <v>2021-04-14</v>
       </c>
       <c r="S3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-01</v>
+        <v>2021-04-15</v>
       </c>
       <c r="T3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-02</v>
+        <v>2021-04-16</v>
       </c>
       <c r="U3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-03</v>
+        <v>2021-04-17</v>
       </c>
       <c r="V3" s="61" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-04</v>
+        <v>2021-04-18</v>
       </c>
       <c r="W3" s="59" t="d">
         <f>V3+1</f>
-        <v>2021-04-05</v>
+        <v>2021-04-19</v>
       </c>
       <c r="X3" s="60" t="d">
         <f>W3+1</f>
-        <v>2021-04-06</v>
+        <v>2021-04-20</v>
       </c>
       <c r="Y3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-07</v>
+        <v>2021-04-21</v>
       </c>
       <c r="Z3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-08</v>
+        <v>2021-04-22</v>
       </c>
       <c r="AA3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-09</v>
+        <v>2021-04-23</v>
       </c>
       <c r="AB3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-10</v>
+        <v>2021-04-24</v>
       </c>
       <c r="AC3" s="61" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-11</v>
+        <v>2021-04-25</v>
       </c>
       <c r="AD3" s="59" t="d">
         <f>AC3+1</f>
-        <v>2021-04-12</v>
+        <v>2021-04-26</v>
       </c>
       <c r="AE3" s="60" t="d">
         <f>AD3+1</f>
-        <v>2021-04-13</v>
+        <v>2021-04-27</v>
       </c>
       <c r="AF3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-14</v>
+        <v>2021-04-28</v>
       </c>
       <c r="AG3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-15</v>
+        <v>2021-04-29</v>
       </c>
       <c r="AH3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-16</v>
+        <v>2021-04-30</v>
       </c>
       <c r="AI3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-17</v>
+        <v>2021-05-01</v>
       </c>
       <c r="AJ3" s="61" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-18</v>
+        <v>2021-05-02</v>
       </c>
       <c r="AK3" s="59" t="d">
         <f>AJ3+1</f>
-        <v>2021-04-19</v>
+        <v>2021-05-03</v>
       </c>
       <c r="AL3" s="60" t="d">
         <f>AK3+1</f>
-        <v>2021-04-20</v>
+        <v>2021-05-04</v>
       </c>
       <c r="AM3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-21</v>
+        <v>2021-05-05</v>
       </c>
       <c r="AN3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-22</v>
+        <v>2021-05-06</v>
       </c>
       <c r="AO3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-23</v>
+        <v>2021-05-07</v>
       </c>
       <c r="AP3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-24</v>
+        <v>2021-05-08</v>
       </c>
       <c r="AQ3" s="61" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-25</v>
+        <v>2021-05-09</v>
       </c>
       <c r="AR3" s="59" t="d">
         <f>AQ3+1</f>
-        <v>2021-04-26</v>
+        <v>2021-05-10</v>
       </c>
       <c r="AS3" s="60" t="d">
         <f>AR3+1</f>
-        <v>2021-04-27</v>
+        <v>2021-05-11</v>
       </c>
       <c r="AT3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-28</v>
+        <v>2021-05-12</v>
       </c>
       <c r="AU3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-29</v>
+        <v>2021-05-13</v>
       </c>
       <c r="AV3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-04-30</v>
+        <v>2021-05-14</v>
       </c>
       <c r="AW3" s="60" t="d">
         <f t="shared" si="0"/>
-        <v>2021-05-01</v>
+        <v>2021-05-15</v>
       </c>
       <c r="AX3" s="61" t="d">
         <f t="shared" si="0"/>
-        <v>2021-05-02</v>
+        <v>2021-05-16</v>
       </c>
       <c r="AY3" s="59" t="d">
         <f>AX3+1</f>
-        <v>2021-05-03</v>
+        <v>2021-05-17</v>
       </c>
       <c r="AZ3" s="60" t="d">
         <f>AY3+1</f>
-        <v>2021-05-04</v>
+        <v>2021-05-18</v>
       </c>
       <c r="BA3" s="60" t="d">
         <f t="shared" ref="BA3:BE3" si="1">AZ3+1</f>
-        <v>2021-05-05</v>
+        <v>2021-05-19</v>
       </c>
       <c r="BB3" s="60" t="d">
         <f t="shared" si="1"/>
-        <v>2021-05-06</v>
+        <v>2021-05-20</v>
       </c>
       <c r="BC3" s="60" t="d">
         <f t="shared" si="1"/>
-        <v>2021-05-07</v>
+        <v>2021-05-21</v>
       </c>
       <c r="BD3" s="60" t="d">
         <f t="shared" si="1"/>
-        <v>2021-05-08</v>
+        <v>2021-05-22</v>
       </c>
       <c r="BE3" s="61" t="d">
         <f t="shared" si="1"/>
-        <v>2021-05-09</v>
+        <v>2021-05-23</v>
       </c>
       <c r="BF3" s="59" t="d">
         <f>BE3+1</f>
-        <v>2021-05-10</v>
+        <v>2021-05-24</v>
       </c>
       <c r="BG3" s="60" t="d">
         <f>BF3+1</f>
-        <v>2021-05-11</v>
+        <v>2021-05-25</v>
       </c>
       <c r="BH3" s="60" t="d">
         <f t="shared" ref="BH3:BL3" si="2">BG3+1</f>
-        <v>2021-05-12</v>
+        <v>2021-05-26</v>
       </c>
       <c r="BI3" s="60" t="d">
         <f t="shared" si="2"/>
-        <v>2021-05-13</v>
+        <v>2021-05-27</v>
       </c>
       <c r="BJ3" s="60" t="d">
         <f t="shared" si="2"/>
-        <v>2021-05-14</v>
+        <v>2021-05-28</v>
       </c>
       <c r="BK3" s="60" t="d">
         <f t="shared" si="2"/>
-        <v>2021-05-15</v>
+        <v>2021-05-29</v>
       </c>
       <c r="BL3" s="61" t="d">
         <f t="shared" si="2"/>
-        <v>2021-05-16</v>
+        <v>2021-05-30</v>
       </c>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1">
@@ -2318,20 +2315,20 @@
       <c r="BL5" s="29"/>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1">
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="96" t="s">
+      <c r="C6" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="97">
+      <c r="D6" s="96">
         <v>1</v>
       </c>
-      <c r="E6" s="98" t="d">
+      <c r="E6" s="97" t="d">
         <f>DATE(2021, 3, 10)</f>
         <v>2021-03-10</v>
       </c>
-      <c r="F6" s="98" t="d">
+      <c r="F6" s="97" t="d">
         <f>DATE(2021, 3, 13)</f>
         <v>2021-03-13</v>
       </c>
@@ -2393,20 +2390,20 @@
       <c r="BL6" s="29"/>
     </row>
     <row r="7" spans="1:64" ht="30" customHeight="1">
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="96" t="s">
+      <c r="C7" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="97">
+      <c r="D7" s="96">
         <v>1</v>
       </c>
-      <c r="E7" s="98" t="d">
+      <c r="E7" s="97" t="d">
         <f>DATE(2021, 3, 14)</f>
         <v>2021-03-14</v>
       </c>
-      <c r="F7" s="98" t="d">
+      <c r="F7" s="97" t="d">
         <f>DATE(2021, 3, 20)</f>
         <v>2021-03-20</v>
       </c>
@@ -2480,7 +2477,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8" t="str">
-        <f t="shared" ref="H8:H41" ca="1" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H40" ca="1" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="29"/>
@@ -2558,13 +2555,13 @@
         <v>2021-03-21</v>
       </c>
       <c r="F9" s="67" t="d">
-        <f>DATE(2021, 3, 27)</f>
-        <v>2021-03-27</v>
+        <f>DATE(2021, 4, 2)</f>
+        <v>2021-04-02</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I9" s="29"/>
       <c r="J9" s="29"/>
@@ -2627,27 +2624,27 @@
       <c r="A10" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="94" t="s">
+      <c r="B10" s="93" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D10" s="13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E10" s="67" t="d">
-        <f>DATE(2021, 3, 28)</f>
-        <v>2021-03-28</v>
-      </c>
-      <c r="F10" s="67" t="d">
         <f>DATE(2021, 4, 3)</f>
         <v>2021-04-03</v>
+      </c>
+      <c r="F10" s="67" t="d">
+        <f>DATE(2021, 4, 6)</f>
+        <v>2021-04-06</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I10" s="29"/>
       <c r="J10" s="29"/>
@@ -2709,17 +2706,17 @@
     <row r="11" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A11" s="42"/>
       <c r="B11" s="58" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D11" s="13">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E11" s="67" t="d">
-        <f>DATE(2021, 4, 4)</f>
-        <v>2021-04-04</v>
+        <f>DATE(2021, 4, 3)</f>
+        <v>2021-04-03</v>
       </c>
       <c r="F11" s="67" t="d">
         <f>DATE(2021, 4, 10)</f>
@@ -2728,7 +2725,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I11" s="29"/>
       <c r="J11" s="29"/>
@@ -2790,7 +2787,7 @@
     <row r="12" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A12" s="42"/>
       <c r="B12" s="58" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C12" s="48" t="s">
         <v>21</v>
@@ -2868,7 +2865,7 @@
     <row r="13" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A13" s="42"/>
       <c r="B13" s="58" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="48" t="s">
         <v>21</v>
@@ -2946,7 +2943,7 @@
     <row r="14" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A14" s="42"/>
       <c r="B14" s="58" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C14" s="48" t="s">
         <v>21</v>
@@ -3024,7 +3021,7 @@
     <row r="15" spans="1:64" s="2" customFormat="1" ht="39.75" customHeight="1">
       <c r="A15" s="42"/>
       <c r="B15" s="57" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C15" s="48" t="s">
         <v>21</v>
@@ -3101,10 +3098,10 @@
     </row>
     <row r="16" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A16" s="43" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="15"/>
@@ -3175,26 +3172,26 @@
     <row r="17" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="43"/>
       <c r="B17" s="79" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D17" s="16">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E17" s="70" t="d">
         <f>DATE(2021, 3, 21)</f>
         <v>2021-03-21</v>
       </c>
       <c r="F17" s="70" t="d">
-        <f>E17+6</f>
-        <v>2021-03-27</v>
+        <f>DATE(2021, 4, 9)</f>
+        <v>2021-04-09</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I17" s="29"/>
       <c r="J17" s="29"/>
@@ -3256,26 +3253,26 @@
     <row r="18" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A18" s="42"/>
       <c r="B18" s="78" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D18" s="16">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E18" s="70" t="d">
-        <f>E17+7</f>
-        <v>2021-03-28</v>
+        <f>DATE(2021, 4, 8)</f>
+        <v>2021-04-08</v>
       </c>
       <c r="F18" s="70" t="d">
-        <f>E18+6</f>
-        <v>2021-04-03</v>
+        <f>E18+9</f>
+        <v>2021-04-17</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I18" s="29"/>
       <c r="J18" s="29"/>
@@ -3337,26 +3334,26 @@
     <row r="19" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A19" s="42"/>
       <c r="B19" s="78" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D19" s="16">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="E19" s="70" t="d">
-        <f>E18</f>
-        <v>2021-03-28</v>
+        <f>DATE(2021, 3, 29)</f>
+        <v>2021-03-29</v>
       </c>
       <c r="F19" s="70" t="d">
-        <f>E19+6</f>
-        <v>2021-04-03</v>
+        <f>DATE(2021, 4, 11)</f>
+        <v>2021-04-11</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I19" s="29"/>
       <c r="J19" s="29"/>
@@ -3418,21 +3415,21 @@
     <row r="20" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="78" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D20" s="16">
         <v>0</v>
       </c>
       <c r="E20" s="70" t="d">
         <f>E19+7</f>
-        <v>2021-04-04</v>
+        <v>2021-04-05</v>
       </c>
       <c r="F20" s="70" t="d">
         <f>E20+6</f>
-        <v>2021-04-10</v>
+        <v>2021-04-11</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8">
@@ -3499,21 +3496,21 @@
     <row r="21" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A21" s="42"/>
       <c r="B21" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="50" t="s">
         <v>38</v>
-      </c>
-      <c r="C21" s="50" t="s">
-        <v>36</v>
       </c>
       <c r="D21" s="16">
         <v>0</v>
       </c>
       <c r="E21" s="70" t="d">
         <f>E20</f>
-        <v>2021-04-04</v>
+        <v>2021-04-05</v>
       </c>
       <c r="F21" s="70" t="d">
         <f>E21+6</f>
-        <v>2021-04-10</v>
+        <v>2021-04-11</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -3577,21 +3574,21 @@
     <row r="22" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="42"/>
       <c r="B22" s="77" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C22" s="80" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D22" s="16">
         <v>0</v>
       </c>
       <c r="E22" s="70" t="d">
-        <f t="shared" ref="E21:E22" si="7">E21+7</f>
-        <v>2021-04-11</v>
+        <f>DATE(2021, 4, 19)</f>
+        <v>2021-04-19</v>
       </c>
       <c r="F22" s="70" t="d">
-        <f t="shared" ref="F21:F22" si="8">E22+6</f>
-        <v>2021-04-17</v>
+        <f>DATE(2021, 4, 28)</f>
+        <v>2021-04-28</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -3655,19 +3652,21 @@
     <row r="23" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="42"/>
       <c r="B23" s="78" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C23" s="77" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D23" s="16">
         <v>0</v>
       </c>
       <c r="E23" s="70" t="d">
-        <v>2021-04-18</v>
+        <f>DATE(2021, 4, 29)</f>
+        <v>2021-04-29</v>
       </c>
       <c r="F23" s="70" t="d">
-        <v>2021-04-24</v>
+        <f>DATE(2021, 5, 6)</f>
+        <v>2021-05-06</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -3731,21 +3730,21 @@
     <row r="24" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A24" s="42"/>
       <c r="B24" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="77" t="s">
         <v>42</v>
-      </c>
-      <c r="C24" s="77" t="s">
-        <v>40</v>
       </c>
       <c r="D24" s="16">
         <v>0</v>
       </c>
       <c r="E24" s="70" t="d">
-        <f>DATE(2021, 4, 25)</f>
-        <v>2021-04-25</v>
+        <f>DATE(2021, 5, 5)</f>
+        <v>2021-05-05</v>
       </c>
       <c r="F24" s="70" t="d">
-        <f>DATE(2021, 5, 1)</f>
-        <v>2021-05-01</v>
+        <f>DATE(2021, 5, 10)</f>
+        <v>2021-05-10</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -3809,21 +3808,21 @@
     <row r="25" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A25" s="42"/>
       <c r="B25" s="78" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C25" s="77" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D25" s="16">
         <v>0</v>
       </c>
       <c r="E25" s="70" t="d">
-        <f>DATE(2021, 5, 2)</f>
-        <v>2021-05-02</v>
+        <f>DATE(2021, 5, 11)</f>
+        <v>2021-05-11</v>
       </c>
       <c r="F25" s="70" t="d">
-        <f>DATE(2021, 5, 15)</f>
-        <v>2021-05-15</v>
+        <f>DATE(2021, 5, 19)</f>
+        <v>2021-05-19</v>
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -3886,10 +3885,10 @@
     </row>
     <row r="26" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A26" s="42" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C26" s="51"/>
       <c r="D26" s="18"/>
@@ -3960,26 +3959,26 @@
     <row r="27" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A27" s="42"/>
       <c r="B27" s="84" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C27" s="52" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D27" s="19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E27" s="73" t="d">
         <f>DATE(2021,3,28)</f>
         <v>2021-03-28</v>
       </c>
       <c r="F27" s="73" t="d">
-        <f>E27+6</f>
-        <v>2021-04-03</v>
+        <f>DATE(2021, 4, 7)</f>
+        <v>2021-04-07</v>
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I27" s="29"/>
       <c r="J27" s="29"/>
@@ -4041,21 +4040,21 @@
     <row r="28" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A28" s="42"/>
       <c r="B28" s="81" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C28" s="52" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D28" s="19">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E28" s="73" t="d">
-        <f>DATE(2021, 4, 4)</f>
-        <v>2021-04-04</v>
+        <f>DATE(2021, 4, 8)</f>
+        <v>2021-04-08</v>
       </c>
       <c r="F28" s="73" t="d">
         <f>E28+6</f>
-        <v>2021-04-10</v>
+        <v>2021-04-14</v>
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="8">
@@ -4122,21 +4121,21 @@
     <row r="29" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A29" s="42"/>
       <c r="B29" s="81" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="52" t="s">
-        <v>47</v>
-      </c>
       <c r="D29" s="19">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E29" s="73" t="d">
         <f>E28+7</f>
-        <v>2021-04-11</v>
+        <v>2021-04-15</v>
       </c>
       <c r="F29" s="73" t="d">
         <f>E29+6</f>
-        <v>2021-04-17</v>
+        <v>2021-04-21</v>
       </c>
       <c r="G29" s="8"/>
       <c r="H29" s="8">
@@ -4203,21 +4202,21 @@
     <row r="30" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A30" s="42"/>
       <c r="B30" s="81" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D30" s="19">
         <v>0</v>
       </c>
       <c r="E30" s="73" t="d">
         <f>F29+1</f>
-        <v>2021-04-18</v>
+        <v>2021-04-22</v>
       </c>
       <c r="F30" s="73" t="d">
         <f>E30+6</f>
-        <v>2021-04-24</v>
+        <v>2021-04-28</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="8">
@@ -4284,10 +4283,10 @@
     <row r="31" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A31" s="42"/>
       <c r="B31" s="81" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C31" s="82" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D31" s="19">
         <v>0</v>
@@ -4362,10 +4361,10 @@
     <row r="32" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A32" s="42"/>
       <c r="B32" s="81" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C32" s="82" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D32" s="19">
         <v>0</v>
@@ -4442,10 +4441,10 @@
     </row>
     <row r="33" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A33" s="42" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B33" s="85" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C33" s="86"/>
       <c r="D33" s="87"/>
@@ -4516,13 +4515,13 @@
     <row r="34" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A34" s="42"/>
       <c r="B34" s="89" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C34" s="90" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D34" s="91">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E34" s="92" t="d">
         <f>DATE(2021, 3, 28)</f>
@@ -4593,23 +4592,13 @@
     </row>
     <row r="35" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A35" s="42"/>
-      <c r="B35" s="93" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="90" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="91">
-        <v>0.6</v>
-      </c>
-      <c r="E35" s="92" t="d">
-        <f>DATE(2021, 3, 29)</f>
-        <v>2021-03-29</v>
-      </c>
-      <c r="F35" s="92" t="d">
-        <f>DATE(2021, 4, 2)</f>
-        <v>2021-04-02</v>
-      </c>
+      <c r="B35" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="53"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="74"/>
+      <c r="F35" s="75"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="29"/>
@@ -4671,13 +4660,23 @@
     </row>
     <row r="36" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A36" s="42"/>
-      <c r="B36" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="75"/>
+      <c r="B36" s="83" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="22">
+        <v>0</v>
+      </c>
+      <c r="E36" s="76" t="d">
+        <f>DATE(2021, 5, 16)</f>
+        <v>2021-05-16</v>
+      </c>
+      <c r="F36" s="76" t="d">
+        <f>DATE(2021, 5, 29)</f>
+        <v>2021-05-29</v>
+      </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="29"/>
@@ -4740,7 +4739,7 @@
     <row r="37" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A37" s="42"/>
       <c r="B37" s="83" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C37" s="54" t="s">
         <v>15</v>
@@ -4749,15 +4748,18 @@
         <v>0</v>
       </c>
       <c r="E37" s="76" t="d">
-        <f>DATE(2021, 5, 16)</f>
-        <v>2021-05-16</v>
+        <f>DATE(2021, 5, 30)</f>
+        <v>2021-05-30</v>
       </c>
       <c r="F37" s="76" t="d">
-        <f>DATE(2021, 5, 29)</f>
-        <v>2021-05-29</v>
+        <f>DATE(2021, 6, 12)</f>
+        <v>2021-06-12</v>
       </c>
       <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
+      <c r="H37" s="8">
+        <f t="shared" ca="1" si="6"/>
+        <v>14</v>
+      </c>
       <c r="I37" s="29"/>
       <c r="J37" s="29"/>
       <c r="K37" s="29"/>
@@ -4818,7 +4820,7 @@
     <row r="38" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A38" s="42"/>
       <c r="B38" s="83" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C38" s="54" t="s">
         <v>15</v>
@@ -4827,17 +4829,17 @@
         <v>0</v>
       </c>
       <c r="E38" s="76" t="d">
-        <f>DATE(2021, 5, 30)</f>
-        <v>2021-05-30</v>
+        <f>DATE(2021, 6, 13)</f>
+        <v>2021-06-13</v>
       </c>
       <c r="F38" s="76" t="d">
-        <f>DATE(2021, 6, 12)</f>
-        <v>2021-06-12</v>
+        <f>DATE(2021, 6, 19)</f>
+        <v>2021-06-19</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="I38" s="29"/>
       <c r="J38" s="29"/>
@@ -4897,28 +4899,18 @@
       <c r="BL38" s="29"/>
     </row>
     <row r="39" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A39" s="42"/>
-      <c r="B39" s="83" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="22">
-        <v>0</v>
-      </c>
-      <c r="E39" s="76" t="d">
-        <f>DATE(2021, 6, 13)</f>
-        <v>2021-06-13</v>
-      </c>
-      <c r="F39" s="76" t="d">
-        <f>DATE(2021, 6, 19)</f>
-        <v>2021-06-19</v>
-      </c>
+      <c r="A39" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="56"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="8">
+      <c r="H39" s="8" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v/>
       </c>
       <c r="I39" s="29"/>
       <c r="J39" s="29"/>
@@ -4977,167 +4969,91 @@
       <c r="BK39" s="29"/>
       <c r="BL39" s="29"/>
     </row>
-    <row r="40" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A40" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="55"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8" t="str">
+    <row r="40" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A40" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="24"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28" t="str">
         <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="29"/>
-      <c r="U40" s="29"/>
-      <c r="V40" s="29"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="29"/>
-      <c r="AC40" s="29"/>
-      <c r="AD40" s="29"/>
-      <c r="AE40" s="29"/>
-      <c r="AF40" s="29"/>
-      <c r="AG40" s="29"/>
-      <c r="AH40" s="29"/>
-      <c r="AI40" s="29"/>
-      <c r="AJ40" s="29"/>
-      <c r="AK40" s="29"/>
-      <c r="AL40" s="29"/>
-      <c r="AM40" s="29"/>
-      <c r="AN40" s="29"/>
-      <c r="AO40" s="29"/>
-      <c r="AP40" s="29"/>
-      <c r="AQ40" s="29"/>
-      <c r="AR40" s="29"/>
-      <c r="AS40" s="29"/>
-      <c r="AT40" s="29"/>
-      <c r="AU40" s="29"/>
-      <c r="AV40" s="29"/>
-      <c r="AW40" s="29"/>
-      <c r="AX40" s="29"/>
-      <c r="AY40" s="29"/>
-      <c r="AZ40" s="29"/>
-      <c r="BA40" s="29"/>
-      <c r="BB40" s="29"/>
-      <c r="BC40" s="29"/>
-      <c r="BD40" s="29"/>
-      <c r="BE40" s="29"/>
-      <c r="BF40" s="29"/>
-      <c r="BG40" s="29"/>
-      <c r="BH40" s="29"/>
-      <c r="BI40" s="29"/>
-      <c r="BJ40" s="29"/>
-      <c r="BK40" s="29"/>
-      <c r="BL40" s="29"/>
-    </row>
-    <row r="41" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A41" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="I41" s="31"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="31"/>
-      <c r="P41" s="31"/>
-      <c r="Q41" s="31"/>
-      <c r="R41" s="31"/>
-      <c r="S41" s="31"/>
-      <c r="T41" s="31"/>
-      <c r="U41" s="31"/>
-      <c r="V41" s="31"/>
-      <c r="W41" s="31"/>
-      <c r="X41" s="31"/>
-      <c r="Y41" s="31"/>
-      <c r="Z41" s="31"/>
-      <c r="AA41" s="31"/>
-      <c r="AB41" s="31"/>
-      <c r="AC41" s="31"/>
-      <c r="AD41" s="31"/>
-      <c r="AE41" s="31"/>
-      <c r="AF41" s="31"/>
-      <c r="AG41" s="31"/>
-      <c r="AH41" s="31"/>
-      <c r="AI41" s="31"/>
-      <c r="AJ41" s="31"/>
-      <c r="AK41" s="31"/>
-      <c r="AL41" s="31"/>
-      <c r="AM41" s="31"/>
-      <c r="AN41" s="31"/>
-      <c r="AO41" s="31"/>
-      <c r="AP41" s="31"/>
-      <c r="AQ41" s="31"/>
-      <c r="AR41" s="31"/>
-      <c r="AS41" s="31"/>
-      <c r="AT41" s="31"/>
-      <c r="AU41" s="31"/>
-      <c r="AV41" s="31"/>
-      <c r="AW41" s="31"/>
-      <c r="AX41" s="31"/>
-      <c r="AY41" s="31"/>
-      <c r="AZ41" s="31"/>
-      <c r="BA41" s="31"/>
-      <c r="BB41" s="31"/>
-      <c r="BC41" s="31"/>
-      <c r="BD41" s="31"/>
-      <c r="BE41" s="31"/>
-      <c r="BF41" s="31"/>
-      <c r="BG41" s="31"/>
-      <c r="BH41" s="31"/>
-      <c r="BI41" s="31"/>
-      <c r="BJ41" s="31"/>
-      <c r="BK41" s="31"/>
-      <c r="BL41" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="31"/>
+      <c r="R40" s="31"/>
+      <c r="S40" s="31"/>
+      <c r="T40" s="31"/>
+      <c r="U40" s="31"/>
+      <c r="V40" s="31"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="31"/>
+      <c r="Y40" s="31"/>
+      <c r="Z40" s="31"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="31"/>
+      <c r="AC40" s="31"/>
+      <c r="AD40" s="31"/>
+      <c r="AE40" s="31"/>
+      <c r="AF40" s="31"/>
+      <c r="AG40" s="31"/>
+      <c r="AH40" s="31"/>
+      <c r="AI40" s="31"/>
+      <c r="AJ40" s="31"/>
+      <c r="AK40" s="31"/>
+      <c r="AL40" s="31"/>
+      <c r="AM40" s="31"/>
+      <c r="AN40" s="31"/>
+      <c r="AO40" s="31"/>
+      <c r="AP40" s="31"/>
+      <c r="AQ40" s="31"/>
+      <c r="AR40" s="31"/>
+      <c r="AS40" s="31"/>
+      <c r="AT40" s="31"/>
+      <c r="AU40" s="31"/>
+      <c r="AV40" s="31"/>
+      <c r="AW40" s="31"/>
+      <c r="AX40" s="31"/>
+      <c r="AY40" s="31"/>
+      <c r="AZ40" s="31"/>
+      <c r="BA40" s="31"/>
+      <c r="BB40" s="31"/>
+      <c r="BC40" s="31"/>
+      <c r="BD40" s="31"/>
+      <c r="BE40" s="31"/>
+      <c r="BF40" s="31"/>
+      <c r="BG40" s="31"/>
+      <c r="BH40" s="31"/>
+      <c r="BI40" s="31"/>
+      <c r="BJ40" s="31"/>
+      <c r="BK40" s="31"/>
+      <c r="BL40" s="31"/>
+    </row>
+    <row r="41" spans="1:64" ht="30" customHeight="1">
+      <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:64" ht="30" customHeight="1">
-      <c r="G42" s="4"/>
+      <c r="C42" s="5"/>
+      <c r="F42" s="44"/>
     </row>
     <row r="43" spans="1:64" ht="30" customHeight="1">
-      <c r="C43" s="5"/>
-      <c r="F43" s="44"/>
-    </row>
-    <row r="44" spans="1:64" ht="30" customHeight="1">
-      <c r="C44" s="6"/>
+      <c r="C43" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="AK2:AQ2"/>
-    <mergeCell ref="AR2:AX2"/>
     <mergeCell ref="AY2:BE2"/>
     <mergeCell ref="BF2:BL2"/>
     <mergeCell ref="E1:F1"/>
@@ -5145,8 +5061,13 @@
     <mergeCell ref="P2:V2"/>
     <mergeCell ref="W2:AC2"/>
     <mergeCell ref="AD2:AJ2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="AK2:AQ2"/>
+    <mergeCell ref="AR2:AX2"/>
   </mergeCells>
-  <conditionalFormatting sqref="D5:D23 D25:D32 D38:D41 D36">
+  <conditionalFormatting sqref="D5:D23 D25:D32 D37:D40 D35">
     <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5160,12 +5081,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:BL41">
+  <conditionalFormatting sqref="I3:BL40">
     <cfRule type="expression" dxfId="2" priority="39">
       <formula>AND(TODAY()&gt;=I$3,TODAY()&lt;J$3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL41">
+  <conditionalFormatting sqref="I5:BL40">
     <cfRule type="expression" dxfId="1" priority="33">
       <formula>AND(task_start&lt;=I$3,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$3)</formula>
     </cfRule>
@@ -5187,7 +5108,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
+  <conditionalFormatting sqref="D36">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5229,20 +5150,6 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.249977111117893"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{02120514-0950-4401-9F0E-EB54624213D2}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="E2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
@@ -5270,7 +5177,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D5:D23 D25:D32 D38:D41 D36</xm:sqref>
+          <xm:sqref>D5:D23 D25:D32 D37:D40 D35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{3DDE5457-78AE-43C9-9381-84A2A6CA3758}">
@@ -5300,7 +5207,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D37</xm:sqref>
+          <xm:sqref>D36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{AD39C701-FA6B-4A49-BBD0-591DF2C9314E}">
@@ -5332,21 +5239,6 @@
           </x14:cfRule>
           <xm:sqref>D34</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{02120514-0950-4401-9F0E-EB54624213D2}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D35</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -5457,6 +5349,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003FB3DE8CD752FC47A176FEA1FC4C26FC" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2779ae4d2e5c77854b22c5f482c24c16">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3ce2f453-a8f0-483d-8543-221e577f3027" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0efa12df6f38754abfbabddf32573e5" ns3:_="">
     <xsd:import namespace="3ce2f453-a8f0-483d-8543-221e577f3027"/>
@@ -5602,23 +5509,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B1877C-41E5-4E95-8716-17BCC82E5619}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9928B0A-825A-46AF-BEAD-F89B0CE3C0F4}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5626,5 +5518,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9928B0A-825A-46AF-BEAD-F89B0CE3C0F4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B1877C-41E5-4E95-8716-17BCC82E5619}"/>
 </file>
</xml_diff>